<commit_message>
Updated News from the forest links
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>August 2018</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest--August-2018.html?soid=1102494320279&amp;aid=Gf4GlQCb5ug</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest--January-2019.html?soid=1102494320279&amp;aid=GtYWC4C0xkA</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,13 +458,17 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update News From The Forest Links.xlsx
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>August 2018</t>
   </si>
@@ -33,9 +33,6 @@
     <t>December 2018</t>
   </si>
   <si>
-    <t>January 2018</t>
-  </si>
-  <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest--December-2018.html?soid=1102494320279&amp;aid=fK6oJK411Vs</t>
   </si>
   <si>
@@ -52,6 +49,15 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest--January-2019.html?soid=1102494320279&amp;aid=GtYWC4C0xkA</t>
+  </si>
+  <si>
+    <t>February 2019</t>
+  </si>
+  <si>
+    <t>January 2019</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest--February-2019.html?soid=1102494320279&amp;aid=G6wA1VRQIZg</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +425,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -427,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -435,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,7 +449,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -451,24 +457,33 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added March link to spreadsheet
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>August 2018</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest--February-2019.html?soid=1102494320279&amp;aid=G6wA1VRQIZg</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest--March-2019.html?soid=1102494320279&amp;aid=F2fljFGzYEQ</t>
+  </si>
+  <si>
+    <t>March 2019</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +482,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>

</xml_diff>

<commit_message>
Added April NFTF link to spreadsheet
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>August 2018</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>March 2019</t>
+  </si>
+  <si>
+    <t>April 2019</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest--April-2019.html?soid=1102494320279&amp;aid=oK_3DP6m1cU</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,14 +496,23 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B6" r:id="rId2"/>
     <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Test Services alignment
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>August 2018</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest--April-2019.html?soid=1102494320279&amp;aid=oK_3DP6m1cU</t>
+  </si>
+  <si>
+    <t>May 2019</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---May-2019.html?soid=1102494320279&amp;aid=11jtFPoUhxc</t>
   </si>
 </sst>
 </file>
@@ -114,10 +120,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,15 +513,24 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B6" r:id="rId2"/>
     <hyperlink ref="B7" r:id="rId3"/>
     <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added June link to list
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>August 2018</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest---May-2019.html?soid=1102494320279&amp;aid=11jtFPoUhxc</t>
+  </si>
+  <si>
+    <t>June 2019</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---June-2019.html?soid=1102494320279&amp;aid=qsCq9FpINss</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +527,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
@@ -528,9 +542,10 @@
     <hyperlink ref="B7" r:id="rId3"/>
     <hyperlink ref="B9" r:id="rId4"/>
     <hyperlink ref="B10" r:id="rId5"/>
+    <hyperlink ref="B11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added August and September NFTF
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>August 2018</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>July 2019</t>
+  </si>
+  <si>
+    <t>August 2019</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---August.html?soid=1102494320279&amp;aid=ePsj_Z-h1SI</t>
+  </si>
+  <si>
+    <t>September 2019</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---September.html?soid=1102494320279&amp;aid=TJ5FtWA1WX4</t>
   </si>
 </sst>
 </file>
@@ -441,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,6 +561,22 @@
         <v>22</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
@@ -558,9 +586,11 @@
     <hyperlink ref="B10" r:id="rId5"/>
     <hyperlink ref="B11" r:id="rId6"/>
     <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B13" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added October NFTF Link
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>August 2018</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest---September.html?soid=1102494320279&amp;aid=TJ5FtWA1WX4</t>
+  </si>
+  <si>
+    <t>October 2019</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---October.html?soid=1102494320279&amp;aid=t-ew4tkMBqU</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +583,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
@@ -588,9 +602,10 @@
     <hyperlink ref="B12" r:id="rId7"/>
     <hyperlink ref="B13" r:id="rId8"/>
     <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B15" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added November NFTF link
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>August 2018</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest---October.html?soid=1102494320279&amp;aid=t-ew4tkMBqU</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---November.html?soid=1102494320279&amp;aid=HrqLhIJI5bY</t>
+  </si>
+  <si>
+    <t>November 2019</t>
   </si>
 </sst>
 </file>
@@ -459,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
@@ -591,6 +597,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
@@ -603,9 +617,10 @@
     <hyperlink ref="B13" r:id="rId8"/>
     <hyperlink ref="B14" r:id="rId9"/>
     <hyperlink ref="B15" r:id="rId10"/>
+    <hyperlink ref="B16" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added May and June NFTF links
</commit_message>
<xml_diff>
--- a/News From The Forest Links.xlsx
+++ b/News From The Forest Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>August 2018</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>https://myemail.constantcontact.com/News-From-The-Forest---April.html?soid=1102494320279&amp;aid=xeQ6VZkeNcs</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---May.html?soid=1102494320279&amp;aid=ycB1LWU2Wpk</t>
+  </si>
+  <si>
+    <t>May 2020</t>
+  </si>
+  <si>
+    <t>June 2020</t>
+  </si>
+  <si>
+    <t>https://myemail.constantcontact.com/News-From-The-Forest---June.html?soid=1102494320279&amp;aid=au6GlYTV-AU</t>
   </si>
 </sst>
 </file>
@@ -483,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,6 +657,22 @@
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -663,9 +691,11 @@
     <hyperlink ref="B17" r:id="rId12"/>
     <hyperlink ref="B18" r:id="rId13"/>
     <hyperlink ref="B19" r:id="rId14"/>
+    <hyperlink ref="B20" r:id="rId15"/>
+    <hyperlink ref="B21" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>